<commit_message>
classmethod and staticmethod decorations
</commit_message>
<xml_diff>
--- a/MacV1Buildup/tables/layer_name_mapping_V1.xlsx
+++ b/MacV1Buildup/tables/layer_name_mapping_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simo\Laskenta\PythonUtilities\MacV1Buildup\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D78D76-30A5-4F41-8AB3-319B930A196F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5036943D-2A85-431D-BD16-2A4260B1FAE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="53">
   <si>
     <t>L4A</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>down_mapping3</t>
-  </si>
-  <si>
-    <t>L4CA;L4CB</t>
   </si>
   <si>
     <t xml:space="preserve"> # sub proportion is the assumed  sub layer Ncells from full layer Ncells (about thickness from full layer thickness)</t>
@@ -558,7 +555,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,7 +567,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -588,7 +585,7 @@
         <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -611,7 +608,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -631,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -700,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>32</v>
@@ -708,7 +705,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -723,15 +720,15 @@
         <v>4</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -746,10 +743,10 @@
         <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -881,13 +878,13 @@
         <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1068,7 +1065,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>32</v>
@@ -1091,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>32</v>
@@ -1114,7 +1111,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>32</v>

</xml_diff>